<commit_message>
Deploying to gh-pages from  @ f11ab41fd45a2e1dc99e43de342676d579d80c47 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/11.6.1.1.xlsx
+++ b/en/downloads/data-excel/11.6.1.1.xlsx
@@ -65,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,25 +166,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
     <col min="1" max="3" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +524,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -537,8 +540,9 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -584,8 +588,11 @@
       <c r="O3" s="8">
         <v>2021</v>
       </c>
+      <c r="P3" s="8">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -595,100 +602,107 @@
       <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="13">
         <v>214.64335233400089</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="13">
         <v>223.17286485664306</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="13">
         <v>183.17358892438764</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="13">
         <v>215.12617344044503</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="13">
         <v>178.26040210730025</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="13">
         <v>195.24385752617454</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="13">
         <v>170.94442632238571</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="13">
         <v>165.14394360035669</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="13">
         <v>172.67633487145682</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="14">
         <v>185.05797171560801</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="14">
         <f>N5/N6*1000</f>
         <v>185.91274954506002</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="14">
         <f>O5/O6*1000</f>
         <v>191.02362938681662</v>
       </c>
+      <c r="P4" s="14">
+        <f>P5/P6*1000</f>
+        <v>212.61804618681055</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="15">
         <v>1114.5999999999999</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="15">
         <v>1173.8</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="15">
         <v>980.4</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="15">
         <v>1175.5999999999999</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="15">
         <v>994.9</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="15">
         <v>1113.3</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="15">
         <v>995.7</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="15">
         <v>981.5</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="15">
         <v>1047.8</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="15">
         <v>1147.5999999999999</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="15">
         <v>1175.9000000000001</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="15">
         <v>1229.5999999999999</v>
       </c>
+      <c r="P5" s="15">
+        <v>1339.6</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:16" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="16">
@@ -726,6 +740,9 @@
       </c>
       <c r="O6" s="16">
         <v>6436.9</v>
+      </c>
+      <c r="P6" s="16">
+        <v>6300.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>